<commit_message>
Ajustes filtros y excel Indicadores
</commit_message>
<xml_diff>
--- a/Service.Report/wwwroot/layout/excel/Indicators/CostoTomaListado.xlsx
+++ b/Service.Report/wwwroot/layout/excel/Indicators/CostoTomaListado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Proyectos\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1C316F-276E-4C0A-964E-5F8D245420B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F6AE90-69AB-4B71-9D26-2C6401B6A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="CostosToma" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CostosToma">CostosToma!$A$4:$C$5</definedName>
+    <definedName name="CostosToma">CostosToma!$A$4:$D$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <r>
       <rPr>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>{{item.CostoToma}}</t>
+  </si>
+  <si>
+    <t>Fecha Modificó</t>
+  </si>
+  <si>
+    <t>{{item.FechaModificacion}}</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +603,9 @@
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -611,6 +619,9 @@
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -620,7 +631,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:C4">
+  <conditionalFormatting sqref="A4:D4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Ajustes filtros y excel Reporte Indicadores
</commit_message>
<xml_diff>
--- a/Service.Report/wwwroot/layout/excel/Indicators/CostoTomaListado.xlsx
+++ b/Service.Report/wwwroot/layout/excel/Indicators/CostoTomaListado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Proyectos\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F6AE90-69AB-4B71-9D26-2C6401B6A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F995B611-CB8D-42E1-B151-525631C255E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
     <t>Fecha Modificó</t>
   </si>
   <si>
-    <t>{{item.FechaModificacion}}</t>
+    <t>{{item.FechaMod}}</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>